<commit_message>
Add disagreement analysis scripts and event extraction enhancements
- Introduced `04b_combine_results_find_disagreement.py` to combine results and identify disagreements between event detection models.
- Created a new Jupyter notebook `05_disagreement_analysis.ipynb` for analyzing disagreements and calculating Cohen's Kappa scores.
- Enhanced the `EventExtractor` class in `event_extractor.py` to track event detection times and improve event extraction logic.
- Updated event extraction methods to include additional attributes and handle various event types more effectively.
- Implemented functionality to save disagreement results and analysis outputs in structured formats.
</commit_message>
<xml_diff>
--- a/resources/keyword_dict_annotated.xlsx
+++ b/resources/keyword_dict_annotated.xlsx
@@ -31,7 +31,7 @@
     <t>positive</t>
   </si>
   <si>
-    <t>Alert and Oriented</t>
+    <t>Others</t>
   </si>
   <si>
     <t>alert</t>
@@ -1713,7 +1713,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1725,9 +1725,6 @@
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -2044,11 +2041,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="22.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="59.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="22.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="5" width="59.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
@@ -2111,7 +2108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -2120,7 +2117,7 @@
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>1</v>
       </c>
     </row>

</xml_diff>